<commit_message>
changed the code to run the shinyapp
</commit_message>
<xml_diff>
--- a/data-raw/Cytotoxicity/Experiment_list_v2.xlsx
+++ b/data-raw/Cytotoxicity/Experiment_list_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\ADViSEBioassay\data-raw\Cytotoxicity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0B73AD-50AE-49DA-8CA5-126156B299C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9823A726-A9C5-4735-9911-1FED5FB44D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE7ED86F-D49E-4F45-8301-2EB4D33C9CAF}"/>
   </bookViews>
@@ -3257,7 +3257,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB9FED2-FFDF-5548-B9ED-7BB53D782206}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F469"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3291,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -3311,7 +3310,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -3351,7 +3350,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -3371,7 +3370,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -3391,7 +3390,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>153</v>
       </c>
@@ -3411,7 +3410,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -3471,7 +3470,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -3491,7 +3490,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -3511,7 +3510,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -3531,7 +3530,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -3551,7 +3550,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3571,7 +3570,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -3591,7 +3590,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>165</v>
       </c>
@@ -3611,7 +3610,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>166</v>
       </c>
@@ -3631,7 +3630,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>167</v>
       </c>
@@ -3651,7 +3650,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3671,7 +3670,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3691,7 +3690,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>174</v>
       </c>
@@ -3711,7 +3710,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>175</v>
       </c>
@@ -3731,7 +3730,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>176</v>
       </c>
@@ -3751,7 +3750,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>177</v>
       </c>
@@ -3771,7 +3770,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>168</v>
       </c>
@@ -3811,7 +3810,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>169</v>
       </c>
@@ -3831,7 +3830,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>170</v>
       </c>
@@ -3851,7 +3850,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>151</v>
       </c>
@@ -3871,7 +3870,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -3891,7 +3890,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>172</v>
       </c>
@@ -3911,7 +3910,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>173</v>
       </c>
@@ -3931,7 +3930,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>178</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>187</v>
       </c>
@@ -3971,7 +3970,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>191</v>
       </c>
@@ -3991,7 +3990,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>192</v>
       </c>
@@ -4011,7 +4010,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>193</v>
       </c>
@@ -4031,7 +4030,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -4051,7 +4050,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>188</v>
       </c>
@@ -4071,7 +4070,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>194</v>
       </c>
@@ -4091,7 +4090,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>195</v>
       </c>
@@ -4111,7 +4110,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -4131,7 +4130,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>197</v>
       </c>
@@ -4151,7 +4150,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>198</v>
       </c>
@@ -4171,7 +4170,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>200</v>
       </c>
@@ -4191,7 +4190,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -4211,7 +4210,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>202</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -4251,7 +4250,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>203</v>
       </c>
@@ -4271,7 +4270,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>204</v>
       </c>
@@ -4291,7 +4290,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>190</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>205</v>
       </c>
@@ -4331,7 +4330,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>206</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>199</v>
       </c>
@@ -4371,7 +4370,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>207</v>
       </c>
@@ -4391,7 +4390,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>208</v>
       </c>
@@ -4411,7 +4410,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -4671,7 +4670,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>44</v>
       </c>
@@ -4691,7 +4690,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>45</v>
       </c>
@@ -4711,7 +4710,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>46</v>
       </c>
@@ -4731,7 +4730,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>47</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -4791,7 +4790,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>54</v>
       </c>
@@ -4811,7 +4810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>55</v>
       </c>
@@ -4831,7 +4830,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>49</v>
       </c>
@@ -4851,7 +4850,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>56</v>
       </c>
@@ -4871,7 +4870,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>57</v>
       </c>
@@ -4891,7 +4890,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>58</v>
       </c>
@@ -4911,7 +4910,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -4931,7 +4930,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -4971,7 +4970,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>50</v>
       </c>
@@ -4991,7 +4990,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>59</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>51</v>
       </c>
@@ -5031,7 +5030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>52</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>60</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>61</v>
       </c>
@@ -5091,7 +5090,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -5111,7 +5110,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -5131,7 +5130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>62</v>
       </c>
@@ -5151,7 +5150,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -5171,7 +5170,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>63</v>
       </c>
@@ -5191,7 +5190,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -5211,7 +5210,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>64</v>
       </c>
@@ -5231,7 +5230,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -5251,7 +5250,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -5271,7 +5270,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>89</v>
       </c>
@@ -5291,7 +5290,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -5311,7 +5310,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -5331,7 +5330,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -5351,7 +5350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -5371,7 +5370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>65</v>
       </c>
@@ -5391,7 +5390,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>66</v>
       </c>
@@ -5411,7 +5410,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>67</v>
       </c>
@@ -5431,7 +5430,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>68</v>
       </c>
@@ -5451,7 +5450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>69</v>
       </c>
@@ -5471,7 +5470,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>70</v>
       </c>
@@ -5491,7 +5490,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>91</v>
       </c>
@@ -5511,7 +5510,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>101</v>
       </c>
@@ -5531,7 +5530,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>92</v>
       </c>
@@ -5551,7 +5550,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>93</v>
       </c>
@@ -5571,7 +5570,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>96</v>
       </c>
@@ -5591,7 +5590,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>97</v>
       </c>
@@ -5611,7 +5610,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -5631,7 +5630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>94</v>
       </c>
@@ -5651,7 +5650,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>102</v>
       </c>
@@ -5671,7 +5670,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>103</v>
       </c>
@@ -6411,7 +6410,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>326</v>
       </c>
@@ -6431,7 +6430,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>328</v>
       </c>
@@ -6451,7 +6450,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>329</v>
       </c>
@@ -6471,7 +6470,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>330</v>
       </c>
@@ -6491,7 +6490,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>331</v>
       </c>
@@ -6511,7 +6510,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>332</v>
       </c>
@@ -6531,7 +6530,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>333</v>
       </c>
@@ -6551,7 +6550,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>334</v>
       </c>
@@ -6571,7 +6570,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>335</v>
       </c>
@@ -6591,7 +6590,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>336</v>
       </c>
@@ -6611,7 +6610,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>337</v>
       </c>
@@ -6631,7 +6630,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>338</v>
       </c>
@@ -6651,7 +6650,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>339</v>
       </c>
@@ -6671,7 +6670,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>340</v>
       </c>
@@ -6691,7 +6690,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>341</v>
       </c>
@@ -6711,7 +6710,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>342</v>
       </c>
@@ -6731,7 +6730,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>343</v>
       </c>
@@ -6751,7 +6750,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>344</v>
       </c>
@@ -6771,7 +6770,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>345</v>
       </c>
@@ -6791,7 +6790,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>346</v>
       </c>
@@ -6811,7 +6810,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>347</v>
       </c>
@@ -6831,7 +6830,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>348</v>
       </c>
@@ -6851,7 +6850,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>349</v>
       </c>
@@ -6871,7 +6870,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>350</v>
       </c>
@@ -6891,7 +6890,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>374</v>
       </c>
@@ -6911,7 +6910,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>375</v>
       </c>
@@ -6931,7 +6930,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>376</v>
       </c>
@@ -6951,7 +6950,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>377</v>
       </c>
@@ -6971,7 +6970,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>378</v>
       </c>
@@ -6991,7 +6990,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>379</v>
       </c>
@@ -7011,7 +7010,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>380</v>
       </c>
@@ -7031,7 +7030,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>381</v>
       </c>
@@ -7051,7 +7050,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>382</v>
       </c>
@@ -7071,7 +7070,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>383</v>
       </c>
@@ -7091,7 +7090,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>384</v>
       </c>
@@ -7111,7 +7110,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>385</v>
       </c>
@@ -7131,7 +7130,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>386</v>
       </c>
@@ -7151,7 +7150,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>387</v>
       </c>
@@ -7171,7 +7170,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>388</v>
       </c>
@@ -7191,7 +7190,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>389</v>
       </c>
@@ -7211,7 +7210,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>390</v>
       </c>
@@ -7231,7 +7230,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>391</v>
       </c>
@@ -7251,7 +7250,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>392</v>
       </c>
@@ -7271,7 +7270,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>412</v>
       </c>
@@ -7291,7 +7290,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>413</v>
       </c>
@@ -7311,7 +7310,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>414</v>
       </c>
@@ -7331,7 +7330,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>415</v>
       </c>
@@ -7351,7 +7350,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>416</v>
       </c>
@@ -7371,7 +7370,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>417</v>
       </c>
@@ -7391,7 +7390,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>418</v>
       </c>
@@ -7411,7 +7410,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>419</v>
       </c>
@@ -7431,7 +7430,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>420</v>
       </c>
@@ -7451,7 +7450,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>421</v>
       </c>
@@ -7471,7 +7470,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>422</v>
       </c>
@@ -7491,7 +7490,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>423</v>
       </c>
@@ -7511,7 +7510,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>424</v>
       </c>
@@ -7531,7 +7530,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>425</v>
       </c>
@@ -7551,7 +7550,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>426</v>
       </c>
@@ -7571,7 +7570,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>427</v>
       </c>
@@ -7591,7 +7590,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>428</v>
       </c>
@@ -7611,7 +7610,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>429</v>
       </c>
@@ -7631,7 +7630,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>430</v>
       </c>
@@ -7651,7 +7650,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>431</v>
       </c>
@@ -7671,7 +7670,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>432</v>
       </c>
@@ -7691,7 +7690,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>433</v>
       </c>
@@ -7711,7 +7710,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>434</v>
       </c>
@@ -7731,7 +7730,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>435</v>
       </c>
@@ -7751,7 +7750,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>436</v>
       </c>
@@ -7771,7 +7770,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>437</v>
       </c>
@@ -7791,7 +7790,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>438</v>
       </c>
@@ -7811,7 +7810,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>439</v>
       </c>
@@ -7831,7 +7830,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>440</v>
       </c>
@@ -7851,7 +7850,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>470</v>
       </c>
@@ -7871,7 +7870,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>471</v>
       </c>
@@ -7891,7 +7890,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>472</v>
       </c>
@@ -7911,7 +7910,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>473</v>
       </c>
@@ -7931,7 +7930,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>474</v>
       </c>
@@ -7951,7 +7950,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>475</v>
       </c>
@@ -7971,7 +7970,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>476</v>
       </c>
@@ -7991,7 +7990,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>477</v>
       </c>
@@ -8011,7 +8010,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>478</v>
       </c>
@@ -8031,7 +8030,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>479</v>
       </c>
@@ -8051,7 +8050,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>480</v>
       </c>
@@ -8071,7 +8070,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>481</v>
       </c>
@@ -8091,7 +8090,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>482</v>
       </c>
@@ -8111,7 +8110,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>483</v>
       </c>
@@ -8131,7 +8130,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>484</v>
       </c>
@@ -8151,7 +8150,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>485</v>
       </c>
@@ -8171,7 +8170,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>486</v>
       </c>
@@ -8191,7 +8190,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>487</v>
       </c>
@@ -8211,7 +8210,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>488</v>
       </c>
@@ -8231,7 +8230,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>489</v>
       </c>
@@ -8251,7 +8250,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>490</v>
       </c>
@@ -8271,7 +8270,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>491</v>
       </c>
@@ -8291,7 +8290,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>492</v>
       </c>
@@ -8311,7 +8310,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>493</v>
       </c>
@@ -8331,7 +8330,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>494</v>
       </c>
@@ -8351,7 +8350,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>520</v>
       </c>
@@ -8371,7 +8370,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>521</v>
       </c>
@@ -8391,7 +8390,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>522</v>
       </c>
@@ -8411,7 +8410,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>523</v>
       </c>
@@ -8431,7 +8430,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>524</v>
       </c>
@@ -8451,7 +8450,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>525</v>
       </c>
@@ -8471,7 +8470,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>526</v>
       </c>
@@ -8491,7 +8490,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>527</v>
       </c>
@@ -8511,7 +8510,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>528</v>
       </c>
@@ -8531,7 +8530,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>538</v>
       </c>
@@ -8551,7 +8550,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>539</v>
       </c>
@@ -8571,7 +8570,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>540</v>
       </c>
@@ -8591,7 +8590,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>541</v>
       </c>
@@ -8611,7 +8610,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>542</v>
       </c>
@@ -8631,7 +8630,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>543</v>
       </c>
@@ -8651,7 +8650,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>544</v>
       </c>
@@ -8671,7 +8670,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>545</v>
       </c>
@@ -8691,7 +8690,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>546</v>
       </c>
@@ -8711,7 +8710,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>547</v>
       </c>
@@ -8731,7 +8730,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>548</v>
       </c>
@@ -8751,7 +8750,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>549</v>
       </c>
@@ -8771,7 +8770,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>550</v>
       </c>
@@ -8791,7 +8790,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>551</v>
       </c>
@@ -8811,7 +8810,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>552</v>
       </c>
@@ -8831,7 +8830,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>553</v>
       </c>
@@ -8851,7 +8850,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>554</v>
       </c>
@@ -8871,7 +8870,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>572</v>
       </c>
@@ -8891,7 +8890,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>573</v>
       </c>
@@ -8911,7 +8910,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>574</v>
       </c>
@@ -8931,7 +8930,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>575</v>
       </c>
@@ -8951,7 +8950,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>576</v>
       </c>
@@ -8971,7 +8970,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>577</v>
       </c>
@@ -8991,7 +8990,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>578</v>
       </c>
@@ -9011,7 +9010,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>579</v>
       </c>
@@ -9031,7 +9030,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>580</v>
       </c>
@@ -9051,7 +9050,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>581</v>
       </c>
@@ -9071,7 +9070,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>582</v>
       </c>
@@ -9091,7 +9090,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>583</v>
       </c>
@@ -9111,7 +9110,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>584</v>
       </c>
@@ -9131,7 +9130,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>585</v>
       </c>
@@ -9151,7 +9150,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>586</v>
       </c>
@@ -9171,7 +9170,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>587</v>
       </c>
@@ -9191,7 +9190,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>588</v>
       </c>
@@ -9211,7 +9210,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>589</v>
       </c>
@@ -9231,7 +9230,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>590</v>
       </c>
@@ -9251,7 +9250,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>591</v>
       </c>
@@ -9271,7 +9270,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>592</v>
       </c>
@@ -9291,7 +9290,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>593</v>
       </c>
@@ -9311,7 +9310,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>594</v>
       </c>
@@ -9331,7 +9330,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>595</v>
       </c>
@@ -9351,7 +9350,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>596</v>
       </c>
@@ -9371,7 +9370,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>597</v>
       </c>
@@ -9391,7 +9390,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>598</v>
       </c>
@@ -9411,7 +9410,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>599</v>
       </c>
@@ -9431,7 +9430,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>600</v>
       </c>
@@ -9451,7 +9450,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>601</v>
       </c>
@@ -9471,7 +9470,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>602</v>
       </c>
@@ -9491,7 +9490,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>603</v>
       </c>
@@ -9511,7 +9510,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>604</v>
       </c>
@@ -9531,7 +9530,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>605</v>
       </c>
@@ -9551,7 +9550,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>606</v>
       </c>
@@ -9571,7 +9570,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>607</v>
       </c>
@@ -9591,7 +9590,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>608</v>
       </c>
@@ -9611,7 +9610,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>609</v>
       </c>
@@ -9631,7 +9630,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>610</v>
       </c>
@@ -9651,7 +9650,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>611</v>
       </c>
@@ -9671,7 +9670,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>651</v>
       </c>
@@ -9691,7 +9690,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>652</v>
       </c>
@@ -9711,7 +9710,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>653</v>
       </c>
@@ -9731,7 +9730,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>654</v>
       </c>
@@ -9751,7 +9750,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>655</v>
       </c>
@@ -9771,7 +9770,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>656</v>
       </c>
@@ -9791,7 +9790,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>657</v>
       </c>
@@ -9811,7 +9810,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>658</v>
       </c>
@@ -9831,7 +9830,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>659</v>
       </c>
@@ -9851,7 +9850,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>660</v>
       </c>
@@ -9871,7 +9870,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>661</v>
       </c>
@@ -9891,7 +9890,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>662</v>
       </c>
@@ -9911,7 +9910,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>663</v>
       </c>
@@ -9931,7 +9930,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>664</v>
       </c>
@@ -9951,7 +9950,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>665</v>
       </c>
@@ -9971,7 +9970,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>666</v>
       </c>
@@ -9991,7 +9990,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>667</v>
       </c>
@@ -10011,7 +10010,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>668</v>
       </c>
@@ -10031,7 +10030,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>669</v>
       </c>
@@ -10051,7 +10050,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>670</v>
       </c>
@@ -10071,7 +10070,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>671</v>
       </c>
@@ -10091,7 +10090,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>672</v>
       </c>
@@ -10111,7 +10110,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>673</v>
       </c>
@@ -10131,7 +10130,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>674</v>
       </c>
@@ -10151,7 +10150,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>675</v>
       </c>
@@ -10171,7 +10170,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>676</v>
       </c>
@@ -10191,7 +10190,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>677</v>
       </c>
@@ -10211,7 +10210,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>678</v>
       </c>
@@ -10231,7 +10230,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>679</v>
       </c>
@@ -10251,7 +10250,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>680</v>
       </c>
@@ -10271,7 +10270,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>681</v>
       </c>
@@ -10291,7 +10290,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>682</v>
       </c>
@@ -10311,7 +10310,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>683</v>
       </c>
@@ -10331,7 +10330,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>684</v>
       </c>
@@ -10351,7 +10350,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>685</v>
       </c>
@@ -10371,7 +10370,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>686</v>
       </c>
@@ -10391,7 +10390,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>687</v>
       </c>
@@ -10411,7 +10410,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>688</v>
       </c>
@@ -10431,7 +10430,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>689</v>
       </c>
@@ -10451,7 +10450,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>690</v>
       </c>
@@ -10471,7 +10470,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>691</v>
       </c>
@@ -10491,7 +10490,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>733</v>
       </c>
@@ -10511,7 +10510,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>734</v>
       </c>
@@ -10531,7 +10530,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>735</v>
       </c>
@@ -10551,7 +10550,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>736</v>
       </c>
@@ -10571,7 +10570,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>737</v>
       </c>
@@ -10591,7 +10590,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>738</v>
       </c>
@@ -10611,7 +10610,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>739</v>
       </c>
@@ -10631,7 +10630,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>740</v>
       </c>
@@ -10651,7 +10650,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>741</v>
       </c>
@@ -10671,7 +10670,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>742</v>
       </c>
@@ -10691,7 +10690,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>743</v>
       </c>
@@ -10711,7 +10710,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>744</v>
       </c>
@@ -10731,7 +10730,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>745</v>
       </c>
@@ -10751,7 +10750,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>746</v>
       </c>
@@ -10771,7 +10770,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>747</v>
       </c>
@@ -10791,7 +10790,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>748</v>
       </c>
@@ -10811,7 +10810,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>749</v>
       </c>
@@ -10831,7 +10830,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>750</v>
       </c>
@@ -10851,7 +10850,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>751</v>
       </c>
@@ -10871,7 +10870,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>752</v>
       </c>
@@ -10891,7 +10890,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>753</v>
       </c>
@@ -10911,7 +10910,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>754</v>
       </c>
@@ -10931,7 +10930,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>755</v>
       </c>
@@ -10951,7 +10950,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>756</v>
       </c>
@@ -10971,7 +10970,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>757</v>
       </c>
@@ -10991,7 +10990,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>758</v>
       </c>
@@ -11011,7 +11010,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>759</v>
       </c>
@@ -11031,7 +11030,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>760</v>
       </c>
@@ -11051,7 +11050,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>761</v>
       </c>
@@ -11071,7 +11070,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>762</v>
       </c>
@@ -11091,7 +11090,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>763</v>
       </c>
@@ -11111,7 +11110,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>764</v>
       </c>
@@ -11131,7 +11130,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>765</v>
       </c>
@@ -11151,7 +11150,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>766</v>
       </c>
@@ -11171,7 +11170,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>767</v>
       </c>
@@ -11191,7 +11190,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>768</v>
       </c>
@@ -11211,7 +11210,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>769</v>
       </c>
@@ -11231,7 +11230,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>770</v>
       </c>
@@ -11251,7 +11250,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>771</v>
       </c>
@@ -11271,7 +11270,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>772</v>
       </c>
@@ -11291,7 +11290,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>773</v>
       </c>
@@ -11311,7 +11310,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>774</v>
       </c>
@@ -11331,7 +11330,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>775</v>
       </c>
@@ -11351,7 +11350,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>776</v>
       </c>
@@ -11371,7 +11370,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>777</v>
       </c>
@@ -11391,7 +11390,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>778</v>
       </c>
@@ -11411,7 +11410,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>779</v>
       </c>
@@ -11431,7 +11430,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>780</v>
       </c>
@@ -11451,7 +11450,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>781</v>
       </c>
@@ -11471,7 +11470,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>782</v>
       </c>
@@ -11491,7 +11490,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>783</v>
       </c>
@@ -11511,7 +11510,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="413" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>784</v>
       </c>
@@ -11531,7 +11530,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="414" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>785</v>
       </c>
@@ -11551,7 +11550,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="415" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>786</v>
       </c>
@@ -11571,7 +11570,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="416" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>787</v>
       </c>
@@ -11591,7 +11590,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="417" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>788</v>
       </c>
@@ -11611,7 +11610,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="418" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>789</v>
       </c>
@@ -11631,7 +11630,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="419" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>790</v>
       </c>
@@ -11651,7 +11650,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="420" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>791</v>
       </c>
@@ -11671,7 +11670,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="421" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>792</v>
       </c>
@@ -11691,7 +11690,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="422" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>793</v>
       </c>
@@ -11711,7 +11710,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="423" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>794</v>
       </c>
@@ -11731,7 +11730,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="424" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>795</v>
       </c>
@@ -11751,7 +11750,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="425" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>796</v>
       </c>
@@ -11771,7 +11770,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="426" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>797</v>
       </c>
@@ -11791,7 +11790,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="427" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>798</v>
       </c>
@@ -11811,7 +11810,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="428" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>799</v>
       </c>
@@ -11831,7 +11830,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="429" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>800</v>
       </c>
@@ -11851,7 +11850,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="430" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>801</v>
       </c>
@@ -11871,7 +11870,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="431" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>802</v>
       </c>
@@ -11891,7 +11890,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="432" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>803</v>
       </c>
@@ -11911,7 +11910,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="433" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>804</v>
       </c>
@@ -11931,7 +11930,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="434" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>805</v>
       </c>
@@ -11951,7 +11950,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="435" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>806</v>
       </c>
@@ -11971,7 +11970,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="436" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>807</v>
       </c>
@@ -11991,7 +11990,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="437" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>808</v>
       </c>
@@ -12011,7 +12010,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="438" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>809</v>
       </c>
@@ -12031,7 +12030,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="439" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>810</v>
       </c>
@@ -12051,7 +12050,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="440" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>811</v>
       </c>
@@ -12071,7 +12070,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="441" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>812</v>
       </c>
@@ -12091,7 +12090,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="442" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>813</v>
       </c>
@@ -12111,7 +12110,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="443" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>814</v>
       </c>
@@ -12131,7 +12130,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="444" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>815</v>
       </c>
@@ -12151,7 +12150,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="445" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>816</v>
       </c>
@@ -12171,7 +12170,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="446" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>817</v>
       </c>
@@ -12191,7 +12190,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>818</v>
       </c>
@@ -12211,7 +12210,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="448" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>819</v>
       </c>
@@ -12231,7 +12230,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="449" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>820</v>
       </c>
@@ -12251,7 +12250,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="450" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>821</v>
       </c>
@@ -12271,7 +12270,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="451" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>822</v>
       </c>
@@ -12291,7 +12290,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="452" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>823</v>
       </c>
@@ -12311,7 +12310,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="453" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>915</v>
       </c>
@@ -12331,7 +12330,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="454" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>917</v>
       </c>
@@ -12351,7 +12350,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="455" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>919</v>
       </c>
@@ -12371,7 +12370,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="456" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>921</v>
       </c>
@@ -12391,7 +12390,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="457" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>923</v>
       </c>
@@ -12411,7 +12410,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="458" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>925</v>
       </c>
@@ -12431,7 +12430,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="459" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>927</v>
       </c>
@@ -12451,7 +12450,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="460" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>929</v>
       </c>
@@ -12471,7 +12470,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="461" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>931</v>
       </c>
@@ -12491,7 +12490,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="462" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>933</v>
       </c>
@@ -12511,7 +12510,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="463" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>934</v>
       </c>
@@ -12531,7 +12530,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="464" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>935</v>
       </c>
@@ -12551,7 +12550,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="465" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>936</v>
       </c>
@@ -12571,7 +12570,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="466" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>937</v>
       </c>
@@ -12591,7 +12590,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="467" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>939</v>
       </c>
@@ -12611,7 +12610,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="468" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>940</v>
       </c>
@@ -12631,7 +12630,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="469" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>941</v>
       </c>
@@ -12652,13 +12651,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F469" xr:uid="{ADB9FED2-FFDF-5548-B9ED-7BB53D782206}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="4300_CHROMATE_PLATE_READER"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F469" xr:uid="{ADB9FED2-FFDF-5548-B9ED-7BB53D782206}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>